<commit_message>
Update temp/rh QC check.
</commit_message>
<xml_diff>
--- a/data/raw_data/tick_survival_assay/temp-th loggers quality check.xlsx
+++ b/data/raw_data/tick_survival_assay/temp-th loggers quality check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whalendillon/SERDP_Project/data/raw_data/tick_survival_assay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7678C95-3C69-6D41-A5BA-A93E9C3F01EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C0D13-8D15-0941-8E6F-A61123C57EAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="6440" windowWidth="28040" windowHeight="11560" xr2:uid="{154A9678-F6E4-9F4F-872F-4290751695C2}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="11460" windowHeight="14080" xr2:uid="{154A9678-F6E4-9F4F-872F-4290751695C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -36,9 +36,6 @@
     <t>visit_date</t>
   </si>
   <si>
-    <t>data_quality</t>
-  </si>
-  <si>
     <t>okay</t>
   </si>
   <si>
@@ -82,6 +79,33 @@
   </si>
   <si>
     <t>removed during prior visit</t>
+  </si>
+  <si>
+    <t>flatlined at 1%</t>
+  </si>
+  <si>
+    <t>maybe some questionable areas</t>
+  </si>
+  <si>
+    <t>some flatlines at 1%</t>
+  </si>
+  <si>
+    <t>rh_data_quality</t>
+  </si>
+  <si>
+    <t>flatlined at 1% prior to 1/2</t>
+  </si>
+  <si>
+    <t>flatlined at 1%, replaced with logger that was at plot 18</t>
+  </si>
+  <si>
+    <t>flatlined at 1% from 12/18</t>
+  </si>
+  <si>
+    <t>flatlined at 1% prior to 12/29</t>
+  </si>
+  <si>
+    <t>flatlined at 1% prior to 12/18</t>
   </si>
 </sst>
 </file>
@@ -434,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05CF040-269B-2C4A-99E9-42FAFC4B5BA6}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,10 +481,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -474,10 +498,10 @@
         <v>20381844</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -491,10 +515,10 @@
         <v>20381822</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -508,10 +532,10 @@
         <v>20381821</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -525,10 +549,10 @@
         <v>20381828</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -542,10 +566,10 @@
         <v>20381835</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -559,10 +583,10 @@
         <v>20381834</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -576,7 +600,7 @@
         <v>20381833</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -590,10 +614,10 @@
         <v>20381840</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -607,10 +631,10 @@
         <v>20381825</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -624,7 +648,7 @@
         <v>20381842</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -638,7 +662,7 @@
         <v>20381830</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -652,7 +676,7 @@
         <v>20381838</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -666,7 +690,7 @@
         <v>20381843</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -680,7 +704,7 @@
         <v>20381841</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -694,7 +718,7 @@
         <v>20381839</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -708,7 +732,7 @@
         <v>20381823</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -722,7 +746,7 @@
         <v>20381824</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -733,7 +757,7 @@
         <v>20181213</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,7 +771,7 @@
         <v>20381829</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -761,10 +785,10 @@
         <v>20381827</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -778,7 +802,7 @@
         <v>20381831</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -792,10 +816,10 @@
         <v>20381832</v>
       </c>
       <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
         <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -809,7 +833,7 @@
         <v>20381837</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -823,7 +847,370 @@
         <v>20381826</v>
       </c>
       <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>20190109</v>
+      </c>
+      <c r="C27">
+        <v>20381844</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C28">
+        <v>20381822</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>3</v>
+      </c>
+      <c r="B29" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C29">
+        <v>20381821</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>4</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C30">
+        <v>20381828</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C31">
+        <v>20381835</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C32">
+        <v>20381834</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C33">
+        <v>20381833</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C34">
+        <v>20381840</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C35">
+        <v>20381825</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C36">
+        <v>20381842</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C37">
+        <v>20381830</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C38">
+        <v>20381838</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>13</v>
+      </c>
+      <c r="B39" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C39">
+        <v>20381843</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>14</v>
+      </c>
+      <c r="B40" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C40">
+        <v>20381841</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C41">
+        <v>20381839</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C42">
+        <v>20381823</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>17</v>
+      </c>
+      <c r="B43" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C43" s="1">
+        <v>20381824</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C45">
+        <v>20381829</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>20</v>
+      </c>
+      <c r="B46" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C46">
+        <v>20381827</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>21</v>
+      </c>
+      <c r="B47" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C47">
+        <v>20381831</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C48">
+        <v>20381832</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C49">
+        <v>20381837</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>24</v>
+      </c>
+      <c r="B50" s="1">
+        <v>20190109</v>
+      </c>
+      <c r="C50">
+        <v>20381826</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>